<commit_message>
global variables and get_category_emails
</commit_message>
<xml_diff>
--- a/Virtual Visitas (Responses).xlsx
+++ b/Virtual Visitas (Responses).xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkzr3\VirtualVisitas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22506" windowHeight="8754"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Timestamp</t>
   </si>
@@ -124,64 +132,71 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -371,26 +386,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="1" max="22" width="21.57"/>
+    <col min="1" max="22" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,9 +443,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
-        <v>43896.79063503472</v>
+        <v>43896.790635034718</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -436,7 +454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>43896.791247256944</v>
       </c>
@@ -447,9 +465,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
-        <v>43896.79794025463</v>
+        <v>43896.797940254633</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
@@ -457,8 +475,11 @@
       <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>43896.801594375</v>
       </c>
@@ -469,9 +490,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
-        <v>43896.80201140046</v>
+        <v>43896.802011400461</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -480,7 +501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>43896.810073298606</v>
       </c>
@@ -491,9 +512,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
-        <v>43896.82154048611</v>
+        <v>43896.821540486111</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>23</v>
@@ -501,10 +522,13 @@
       <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="E8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
-        <v>43896.83058003472</v>
+        <v>43896.830580034723</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>25</v>
@@ -512,8 +536,11 @@
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>43897.005486215276</v>
       </c>
@@ -523,10 +550,13 @@
       <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
-        <v>43897.37583556713</v>
+        <v>43897.375835567131</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
@@ -560,6 +590,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
by category go through each category value
</commit_message>
<xml_diff>
--- a/Virtual Visitas (Responses).xlsx
+++ b/Virtual Visitas (Responses).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Timestamp</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Neuroscience</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -453,6 +456,9 @@
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
@@ -464,6 +470,9 @@
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
@@ -476,7 +485,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -489,6 +498,9 @@
       <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
@@ -500,6 +512,9 @@
       <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
@@ -511,6 +526,9 @@
       <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
@@ -551,7 +569,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
groupnum updates, nongmails work?
</commit_message>
<xml_diff>
--- a/Virtual Visitas (Responses).xlsx
+++ b/Virtual Visitas (Responses).xlsx
@@ -15,7 +15,6 @@
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -223,9 +222,6 @@
     <t>Cooking/Baking, Hiking, Writing, Shopping, Other</t>
   </si>
   <si>
-    <t>allachelaeticia@ymail.com</t>
-  </si>
-  <si>
     <t>Laeticia Allache</t>
   </si>
   <si>
@@ -239,13 +235,16 @@
   </si>
   <si>
     <t>Music, Dance, Art, Yoga, Reading, Shopping, Other</t>
+  </si>
+  <si>
+    <t>allachelaeticia@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -256,6 +255,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -275,10 +280,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,8 +292,12 @@
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,7 +518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -954,39 +964,42 @@
       <c r="A17" s="2">
         <v>43901.983182870368</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>